<commit_message>
feat ipv6 network configuration plan
</commit_message>
<xml_diff>
--- a/REDES.xlsx
+++ b/REDES.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandro\Documents\Ingenieria\Redes de Computadoras\Trabajo final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandro\Documents\Ingenieria\Redes de Computadoras\redes-tp-integrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F765F49B-9B14-4BAD-A5FA-1E22A324F9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BB2462-D880-4548-8715-69732A8AF534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{568657D2-FBC9-4BFC-83B1-5AD2AE29FCAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{568657D2-FBC9-4BFC-83B1-5AD2AE29FCAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="115">
   <si>
     <t>Dispositivo</t>
   </si>
@@ -305,6 +306,108 @@
   </si>
   <si>
     <t>(DHCP) 10.0.50.254</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::2</t>
+  </si>
+  <si>
+    <t>/127</t>
+  </si>
+  <si>
+    <t>fe80::</t>
+  </si>
+  <si>
+    <t>link-local</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::</t>
+  </si>
+  <si>
+    <t>fe80::1</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::1</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:2::1</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:2::</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::3</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::4</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::5</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::6</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::7</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::8</t>
+  </si>
+  <si>
+    <t>2001:DB8:0:1::9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001:db8:0:10:: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001:db8:0:50:: </t>
+  </si>
+  <si>
+    <t>/64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001:db8:0:60:: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001:db8:0:30:: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001:db8:0:40:: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001:db8:0:70:: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001:db8:0:20:: </t>
+  </si>
+  <si>
+    <t>2800:110:1010::</t>
+  </si>
+  <si>
+    <t>2800:110:1010::8</t>
+  </si>
+  <si>
+    <t>Autoconfiguracion EUI-64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ---</t>
+  </si>
+  <si>
+    <t>2001:db8:0:60::1</t>
+  </si>
+  <si>
+    <t>2001:db8:0:60::</t>
+  </si>
+  <si>
+    <t>2001:db8:0:50::1</t>
+  </si>
+  <si>
+    <t>2001:db8:0:50::</t>
+  </si>
+  <si>
+    <t>2001:db8:0:70::1</t>
+  </si>
+  <si>
+    <t>2001:db8:0:70::2</t>
   </si>
 </sst>
 </file>
@@ -349,7 +452,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -496,15 +599,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -619,21 +713,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -670,6 +749,104 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -679,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
@@ -690,10 +867,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -706,39 +882,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Énfasis5" xfId="1" builtinId="48"/>
@@ -1074,18 +1283,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067A2B1B-9711-43D5-968B-DE0FD84948F8}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -1098,10 +1307,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1114,17 +1323,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="33" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>255255255252</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -1138,14 +1347,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="5"/>
@@ -1157,16 +1366,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="19">
         <v>255255255252</v>
       </c>
       <c r="F4" s="7"/>
@@ -1177,36 +1386,36 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="41"/>
+      <c r="B5" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>255255255252</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="31" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="41"/>
+      <c r="B6" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>255255255252</v>
       </c>
       <c r="F6" s="7"/>
@@ -1217,36 +1426,36 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
+      <c r="B7" s="33" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="31" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="33" t="s">
         <v>68</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="7"/>
@@ -1258,388 +1467,1071 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="19">
         <v>255255255252</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="41"/>
+      <c r="B10" s="33" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>255255255252</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="22">
         <v>255255255252</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="19">
         <v>255255255252</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="39"/>
+      <c r="B13" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <v>255255255252</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="41"/>
+      <c r="B15" s="33" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <v>255255255252</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="41"/>
+      <c r="B18" s="33" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8" t="s">
+      <c r="A19" s="39"/>
+      <c r="B19" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="22">
         <v>255255255252</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="39"/>
+      <c r="B21" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="22">
         <v>255255255252</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="25">
         <v>100100100100</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="11" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="27" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="11" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="27" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="30">
         <v>255255255240</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="34">
+      <c r="D33" s="30">
         <v>255255255240</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="11" t="s">
         <v>63</v>
       </c>
     </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="42"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="42"/>
+      <c r="B38" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="42"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="42"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="42"/>
+      <c r="B42" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="42"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="42"/>
+      <c r="B44" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="42"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="42"/>
+      <c r="B46" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="42"/>
+      <c r="B47" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="42"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="42"/>
+      <c r="B50" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="42"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="42"/>
+      <c r="B52" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="42"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="42"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="42"/>
+      <c r="B56" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="42"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="42"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="42"/>
+      <c r="B60" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="42"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="42"/>
+      <c r="B62" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="42"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="42"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="42"/>
+      <c r="B66" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="42"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="42"/>
+      <c r="B68" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="42"/>
+      <c r="B69" s="43"/>
+      <c r="C69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="42"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="42"/>
+      <c r="B72" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="42"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E73" s="35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E74" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E75" s="37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E76" s="37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D77" s="46"/>
+      <c r="E77" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D78" s="46"/>
+      <c r="E78" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D79" s="46"/>
+      <c r="E79" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="46"/>
+      <c r="E80" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D81" s="46"/>
+      <c r="E81" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D82" s="46"/>
+      <c r="E82" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" s="46"/>
+      <c r="E83" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E84" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D85" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E85" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="39">
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="A64:A69"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
replace rip for ospf ipv4
</commit_message>
<xml_diff>
--- a/REDES.xlsx
+++ b/REDES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandro\Documents\Ingenieria\Redes de Computadoras\redes-tp-integrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5B60ED-C73A-4FD9-96DF-68A9D973C674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B98AF44-59E0-4FA5-8F01-F1F7FF06465F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{568657D2-FBC9-4BFC-83B1-5AD2AE29FCAB}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{568657D2-FBC9-4BFC-83B1-5AD2AE29FCAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -923,6 +923,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -933,18 +945,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1284,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067A2B1B-9711-43D5-968B-DE0FD84948F8}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62:B63"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1323,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="33" t="s">
@@ -1346,7 +1346,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="33" t="s">
         <v>5</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="43" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="33" t="s">
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="33" t="s">
         <v>6</v>
       </c>
@@ -1407,7 +1407,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="33" t="s">
         <v>5</v>
       </c>
@@ -1426,7 +1426,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="33" t="s">
         <v>67</v>
       </c>
@@ -1447,12 +1447,12 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="33" t="s">
         <v>68</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>44</v>
@@ -1466,7 +1466,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="43" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="33" t="s">
@@ -1489,7 +1489,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="33" t="s">
         <v>7</v>
       </c>
@@ -1501,7 +1501,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="33" t="s">
         <v>5</v>
       </c>
@@ -1513,7 +1513,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="33" t="s">
@@ -1527,7 +1527,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="33" t="s">
         <v>5</v>
       </c>
@@ -1539,7 +1539,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="43" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="33" t="s">
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="33" t="s">
         <v>36</v>
       </c>
@@ -1565,7 +1565,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="33" t="s">
         <v>39</v>
       </c>
@@ -1577,7 +1577,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="33" t="s">
@@ -1591,7 +1591,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="33" t="s">
         <v>38</v>
       </c>
@@ -1603,7 +1603,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="33" t="s">
         <v>39</v>
       </c>
@@ -1615,7 +1615,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="33" t="s">
@@ -1629,7 +1629,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="33" t="s">
         <v>39</v>
       </c>
@@ -1863,10 +1863,10 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="41" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1877,8 +1877,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="44"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="1" t="s">
         <v>86</v>
       </c>
@@ -1887,8 +1887,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="44" t="s">
+      <c r="A38" s="42"/>
+      <c r="B38" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1899,8 +1899,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="44"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="1" t="s">
         <v>83</v>
       </c>
@@ -1909,10 +1909,10 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1923,8 +1923,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="44"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="41"/>
       <c r="C41" s="1" t="s">
         <v>83</v>
       </c>
@@ -1933,8 +1933,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="44" t="s">
+      <c r="A42" s="42"/>
+      <c r="B42" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1945,8 +1945,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="43"/>
-      <c r="B43" s="44"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="1" t="s">
         <v>83</v>
       </c>
@@ -1955,8 +1955,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
-      <c r="B44" s="44" t="s">
+      <c r="A44" s="42"/>
+      <c r="B44" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1967,8 +1967,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="43"/>
-      <c r="B45" s="44"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="1" t="s">
         <v>83</v>
       </c>
@@ -1977,7 +1977,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="43"/>
+      <c r="A46" s="42"/>
       <c r="B46" s="34" t="s">
         <v>67</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
+      <c r="A47" s="42"/>
       <c r="B47" s="34" t="s">
         <v>68</v>
       </c>
@@ -2001,10 +2001,10 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="41" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -2015,8 +2015,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
-      <c r="B49" s="44"/>
+      <c r="A49" s="42"/>
+      <c r="B49" s="41"/>
       <c r="C49" s="1" t="s">
         <v>86</v>
       </c>
@@ -2025,8 +2025,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="43"/>
-      <c r="B50" s="44" t="s">
+      <c r="A50" s="42"/>
+      <c r="B50" s="41" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -2037,8 +2037,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="43"/>
-      <c r="B51" s="44"/>
+      <c r="A51" s="42"/>
+      <c r="B51" s="41"/>
       <c r="C51" s="1" t="s">
         <v>83</v>
       </c>
@@ -2047,8 +2047,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="43"/>
-      <c r="B52" s="44" t="s">
+      <c r="A52" s="42"/>
+      <c r="B52" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -2059,8 +2059,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="43"/>
-      <c r="B53" s="44"/>
+      <c r="A53" s="42"/>
+      <c r="B53" s="41"/>
       <c r="C53" s="1" t="s">
         <v>83</v>
       </c>
@@ -2069,10 +2069,10 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="43" t="s">
+      <c r="A54" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="44" t="s">
+      <c r="B54" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -2083,8 +2083,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="43"/>
-      <c r="B55" s="44"/>
+      <c r="A55" s="42"/>
+      <c r="B55" s="41"/>
       <c r="C55" s="1" t="s">
         <v>86</v>
       </c>
@@ -2093,8 +2093,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="43"/>
-      <c r="B56" s="44" t="s">
+      <c r="A56" s="42"/>
+      <c r="B56" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -2105,8 +2105,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="43"/>
-      <c r="B57" s="44"/>
+      <c r="A57" s="42"/>
+      <c r="B57" s="41"/>
       <c r="C57" s="1" t="s">
         <v>83</v>
       </c>
@@ -2115,10 +2115,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="44" t="s">
+      <c r="B58" s="41" t="s">
         <v>35</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -2129,8 +2129,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="43"/>
-      <c r="B59" s="44"/>
+      <c r="A59" s="42"/>
+      <c r="B59" s="41"/>
       <c r="C59" s="1" t="s">
         <v>83</v>
       </c>
@@ -2139,8 +2139,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="43"/>
-      <c r="B60" s="44" t="s">
+      <c r="A60" s="42"/>
+      <c r="B60" s="41" t="s">
         <v>36</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -2151,8 +2151,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="43"/>
-      <c r="B61" s="44"/>
+      <c r="A61" s="42"/>
+      <c r="B61" s="41"/>
       <c r="C61" s="1" t="s">
         <v>83</v>
       </c>
@@ -2161,8 +2161,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="43"/>
-      <c r="B62" s="44" t="s">
+      <c r="A62" s="42"/>
+      <c r="B62" s="41" t="s">
         <v>39</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -2173,8 +2173,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="43"/>
-      <c r="B63" s="44"/>
+      <c r="A63" s="42"/>
+      <c r="B63" s="41"/>
       <c r="C63" s="1" t="s">
         <v>86</v>
       </c>
@@ -2183,10 +2183,10 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="43" t="s">
+      <c r="A64" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B64" s="44" t="s">
+      <c r="B64" s="41" t="s">
         <v>37</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -2197,8 +2197,8 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="43"/>
-      <c r="B65" s="44"/>
+      <c r="A65" s="42"/>
+      <c r="B65" s="41"/>
       <c r="C65" s="1" t="s">
         <v>83</v>
       </c>
@@ -2207,8 +2207,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="43"/>
-      <c r="B66" s="44" t="s">
+      <c r="A66" s="42"/>
+      <c r="B66" s="41" t="s">
         <v>38</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -2219,8 +2219,8 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="43"/>
-      <c r="B67" s="44"/>
+      <c r="A67" s="42"/>
+      <c r="B67" s="41"/>
       <c r="C67" s="1" t="s">
         <v>83</v>
       </c>
@@ -2229,8 +2229,8 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="43"/>
-      <c r="B68" s="44" t="s">
+      <c r="A68" s="42"/>
+      <c r="B68" s="41" t="s">
         <v>39</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -2241,8 +2241,8 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="43"/>
-      <c r="B69" s="44"/>
+      <c r="A69" s="42"/>
+      <c r="B69" s="41"/>
       <c r="C69" s="1" t="s">
         <v>86</v>
       </c>
@@ -2251,10 +2251,10 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="43" t="s">
+      <c r="A70" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="44" t="s">
+      <c r="B70" s="41" t="s">
         <v>34</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -2265,8 +2265,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="43"/>
-      <c r="B71" s="44"/>
+      <c r="A71" s="42"/>
+      <c r="B71" s="41"/>
       <c r="C71" s="1" t="s">
         <v>83</v>
       </c>
@@ -2275,8 +2275,8 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="43"/>
-      <c r="B72" s="44" t="s">
+      <c r="A72" s="42"/>
+      <c r="B72" s="41" t="s">
         <v>39</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -2287,8 +2287,8 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="43"/>
-      <c r="B73" s="44"/>
+      <c r="A73" s="42"/>
+      <c r="B73" s="41"/>
       <c r="C73" s="1" t="s">
         <v>86</v>
       </c>
@@ -2357,10 +2357,10 @@
       <c r="B77" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C77" s="45" t="s">
+      <c r="C77" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D77" s="46"/>
+      <c r="D77" s="40"/>
       <c r="E77" s="38" t="s">
         <v>108</v>
       </c>
@@ -2372,10 +2372,10 @@
       <c r="B78" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C78" s="45" t="s">
+      <c r="C78" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D78" s="46"/>
+      <c r="D78" s="40"/>
       <c r="E78" s="38" t="s">
         <v>108</v>
       </c>
@@ -2387,10 +2387,10 @@
       <c r="B79" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C79" s="45" t="s">
+      <c r="C79" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D79" s="46"/>
+      <c r="D79" s="40"/>
       <c r="E79" s="38" t="s">
         <v>108</v>
       </c>
@@ -2402,10 +2402,10 @@
       <c r="B80" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C80" s="45" t="s">
+      <c r="C80" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D80" s="46"/>
+      <c r="D80" s="40"/>
       <c r="E80" s="38" t="s">
         <v>108</v>
       </c>
@@ -2417,10 +2417,10 @@
       <c r="B81" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C81" s="45" t="s">
+      <c r="C81" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D81" s="46"/>
+      <c r="D81" s="40"/>
       <c r="E81" s="38" t="s">
         <v>108</v>
       </c>
@@ -2432,10 +2432,10 @@
       <c r="B82" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C82" s="45" t="s">
+      <c r="C82" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D82" s="46"/>
+      <c r="D82" s="40"/>
       <c r="E82" s="38" t="s">
         <v>108</v>
       </c>
@@ -2447,10 +2447,10 @@
       <c r="B83" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C83" s="45" t="s">
+      <c r="C83" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D83" s="46"/>
+      <c r="D83" s="40"/>
       <c r="E83" s="38" t="s">
         <v>108</v>
       </c>
@@ -2491,13 +2491,27 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A64:A69"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A47"/>
@@ -2509,27 +2523,13 @@
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A58:A63"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A64:A69"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>